<commit_message>
enable single and range search, but no buffer for search result
</commit_message>
<xml_diff>
--- a/fake_large.xlsx
+++ b/fake_large.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanZzz\source\repos\spreadsheet_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3636BD-6649-4FF4-84AB-258E20EF8EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E8A29A-73BC-4868-ABC5-11320AABD78C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,12 +32,12 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -67,8 +67,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K493"/>
+  <dimension ref="A1:L511"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A493" workbookViewId="0">
+      <selection activeCell="I508" sqref="I508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -22430,7 +22433,7 @@
         <v>34689.196875000096</v>
       </c>
     </row>
-    <row r="481" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="481" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A481">
         <f t="shared" si="145"/>
         <v>1124</v>
@@ -22476,7 +22479,7 @@
         <v>34664.196875000096</v>
       </c>
     </row>
-    <row r="482" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="482" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A482">
         <f t="shared" si="145"/>
         <v>1127</v>
@@ -22522,7 +22525,7 @@
         <v>34639.196875000096</v>
       </c>
     </row>
-    <row r="483" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="483" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A483">
         <f t="shared" si="145"/>
         <v>1130</v>
@@ -22568,7 +22571,7 @@
         <v>34614.196875000096</v>
       </c>
     </row>
-    <row r="484" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="484" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A484">
         <f t="shared" si="145"/>
         <v>1133</v>
@@ -22614,7 +22617,7 @@
         <v>34589.196875000096</v>
       </c>
     </row>
-    <row r="485" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="485" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A485">
         <f t="shared" si="145"/>
         <v>1136</v>
@@ -22660,7 +22663,7 @@
         <v>34564.196875000096</v>
       </c>
     </row>
-    <row r="486" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="486" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A486">
         <f t="shared" si="145"/>
         <v>1139</v>
@@ -22706,7 +22709,7 @@
         <v>34539.196875000096</v>
       </c>
     </row>
-    <row r="487" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="487" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A487">
         <f t="shared" ref="A487:A492" si="156">A486+3</f>
         <v>1142</v>
@@ -22752,7 +22755,7 @@
         <v>34514.196875000096</v>
       </c>
     </row>
-    <row r="488" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="488" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A488">
         <f t="shared" si="156"/>
         <v>1145</v>
@@ -22798,7 +22801,7 @@
         <v>34489.196875000096</v>
       </c>
     </row>
-    <row r="489" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="489" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A489">
         <f t="shared" si="156"/>
         <v>1148</v>
@@ -22844,7 +22847,7 @@
         <v>34464.196875000096</v>
       </c>
     </row>
-    <row r="490" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="490" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A490">
         <f t="shared" si="156"/>
         <v>1151</v>
@@ -22890,7 +22893,7 @@
         <v>34439.196875000096</v>
       </c>
     </row>
-    <row r="491" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="491" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A491">
         <f t="shared" si="156"/>
         <v>1154</v>
@@ -22936,7 +22939,7 @@
         <v>34414.196875000096</v>
       </c>
     </row>
-    <row r="492" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="492" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A492">
         <f t="shared" si="156"/>
         <v>1157</v>
@@ -22982,50 +22985,861 @@
         <v>34389.196875000096</v>
       </c>
     </row>
-    <row r="493" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="493" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A493">
-        <f>A492-30</f>
-        <v>1127</v>
+        <v>7</v>
       </c>
       <c r="B493">
-        <f t="shared" ref="B493" si="161">B492+3</f>
+        <f t="shared" ref="B493:B511" si="161">B492+3</f>
         <v>1191.3999999999999</v>
       </c>
       <c r="C493">
-        <f t="shared" ref="C493" si="162">C492+3</f>
+        <f t="shared" ref="C493:C511" si="162">C492+3</f>
         <v>1275.4000000000001</v>
       </c>
       <c r="D493">
-        <f t="shared" ref="D493" si="163">D492+3</f>
+        <f t="shared" ref="D493:D511" si="163">D492+3</f>
         <v>1449.4000000000003</v>
       </c>
       <c r="E493">
-        <f t="shared" ref="E493" si="164">E492+3</f>
+        <f t="shared" ref="E493:E511" si="164">E492+3</f>
         <v>1794.3999999999985</v>
       </c>
       <c r="F493">
-        <f t="shared" ref="F493" si="165">F492+3</f>
+        <f t="shared" ref="F493:F511" si="165">F492+3</f>
         <v>2485.8999999999987</v>
       </c>
       <c r="G493">
-        <f t="shared" ref="G493" si="166">G492+3</f>
+        <f t="shared" ref="G493:G511" si="166">G492+3</f>
         <v>3868.150000000006</v>
       </c>
       <c r="H493">
-        <f t="shared" ref="H493" si="167">H492-15</f>
+        <f t="shared" ref="H493:H511" si="167">H492-15</f>
         <v>-422.974999999994</v>
       </c>
       <c r="I493">
-        <f t="shared" ref="I493" si="168">I492-25</f>
+        <f t="shared" ref="I493:I511" si="168">I492-25</f>
         <v>1186.587499999976</v>
       </c>
       <c r="J493">
-        <f t="shared" ref="J493" si="169">J492-20</f>
+        <f t="shared" ref="J493:J511" si="169">J492-20</f>
         <v>14205.806249999976</v>
       </c>
       <c r="K493">
-        <f t="shared" ref="K493" si="170">K492-25</f>
+        <f t="shared" ref="K493:K511" si="170">K492-25</f>
         <v>34364.196875000096</v>
+      </c>
+    </row>
+    <row r="494" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A494">
+        <v>7</v>
+      </c>
+      <c r="B494">
+        <f t="shared" si="161"/>
+        <v>1194.3999999999999</v>
+      </c>
+      <c r="C494">
+        <f t="shared" si="162"/>
+        <v>1278.4000000000001</v>
+      </c>
+      <c r="D494">
+        <f t="shared" si="163"/>
+        <v>1452.4000000000003</v>
+      </c>
+      <c r="E494">
+        <f t="shared" si="164"/>
+        <v>1797.3999999999985</v>
+      </c>
+      <c r="F494">
+        <f t="shared" si="165"/>
+        <v>2488.8999999999987</v>
+      </c>
+      <c r="G494">
+        <f t="shared" si="166"/>
+        <v>3871.150000000006</v>
+      </c>
+      <c r="H494">
+        <f t="shared" si="167"/>
+        <v>-437.974999999994</v>
+      </c>
+      <c r="I494">
+        <f t="shared" si="168"/>
+        <v>1161.587499999976</v>
+      </c>
+      <c r="J494">
+        <f t="shared" si="169"/>
+        <v>14185.806249999976</v>
+      </c>
+      <c r="K494">
+        <f t="shared" si="170"/>
+        <v>34339.196875000096</v>
+      </c>
+    </row>
+    <row r="495" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A495">
+        <v>7</v>
+      </c>
+      <c r="B495">
+        <f t="shared" si="161"/>
+        <v>1197.3999999999999</v>
+      </c>
+      <c r="C495">
+        <f t="shared" si="162"/>
+        <v>1281.4000000000001</v>
+      </c>
+      <c r="D495">
+        <f t="shared" si="163"/>
+        <v>1455.4000000000003</v>
+      </c>
+      <c r="E495">
+        <f t="shared" si="164"/>
+        <v>1800.3999999999985</v>
+      </c>
+      <c r="F495">
+        <f t="shared" si="165"/>
+        <v>2491.8999999999987</v>
+      </c>
+      <c r="G495">
+        <f t="shared" si="166"/>
+        <v>3874.150000000006</v>
+      </c>
+      <c r="H495">
+        <f t="shared" si="167"/>
+        <v>-452.974999999994</v>
+      </c>
+      <c r="I495">
+        <f t="shared" si="168"/>
+        <v>1136.587499999976</v>
+      </c>
+      <c r="J495">
+        <f t="shared" si="169"/>
+        <v>14165.806249999976</v>
+      </c>
+      <c r="K495">
+        <f t="shared" si="170"/>
+        <v>34314.196875000096</v>
+      </c>
+      <c r="L495" s="1"/>
+    </row>
+    <row r="496" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A496">
+        <v>7</v>
+      </c>
+      <c r="B496">
+        <f t="shared" si="161"/>
+        <v>1200.3999999999999</v>
+      </c>
+      <c r="C496">
+        <f t="shared" si="162"/>
+        <v>1284.4000000000001</v>
+      </c>
+      <c r="D496">
+        <f t="shared" si="163"/>
+        <v>1458.4000000000003</v>
+      </c>
+      <c r="E496">
+        <f t="shared" si="164"/>
+        <v>1803.3999999999985</v>
+      </c>
+      <c r="F496">
+        <f t="shared" si="165"/>
+        <v>2494.8999999999987</v>
+      </c>
+      <c r="G496">
+        <f t="shared" si="166"/>
+        <v>3877.150000000006</v>
+      </c>
+      <c r="H496">
+        <f t="shared" si="167"/>
+        <v>-467.974999999994</v>
+      </c>
+      <c r="I496">
+        <f t="shared" si="168"/>
+        <v>1111.587499999976</v>
+      </c>
+      <c r="J496">
+        <f t="shared" si="169"/>
+        <v>14145.806249999976</v>
+      </c>
+      <c r="K496">
+        <f t="shared" si="170"/>
+        <v>34289.196875000096</v>
+      </c>
+    </row>
+    <row r="497" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A497">
+        <v>7</v>
+      </c>
+      <c r="B497">
+        <f t="shared" si="161"/>
+        <v>1203.3999999999999</v>
+      </c>
+      <c r="C497">
+        <f t="shared" si="162"/>
+        <v>1287.4000000000001</v>
+      </c>
+      <c r="D497">
+        <f t="shared" si="163"/>
+        <v>1461.4000000000003</v>
+      </c>
+      <c r="E497">
+        <f t="shared" si="164"/>
+        <v>1806.3999999999985</v>
+      </c>
+      <c r="F497">
+        <f t="shared" si="165"/>
+        <v>2497.8999999999987</v>
+      </c>
+      <c r="G497">
+        <f t="shared" si="166"/>
+        <v>3880.150000000006</v>
+      </c>
+      <c r="H497">
+        <f t="shared" si="167"/>
+        <v>-482.974999999994</v>
+      </c>
+      <c r="I497">
+        <f t="shared" si="168"/>
+        <v>1086.587499999976</v>
+      </c>
+      <c r="J497">
+        <f t="shared" si="169"/>
+        <v>14125.806249999976</v>
+      </c>
+      <c r="K497">
+        <f t="shared" si="170"/>
+        <v>34264.196875000096</v>
+      </c>
+    </row>
+    <row r="498" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A498">
+        <v>7</v>
+      </c>
+      <c r="B498">
+        <f t="shared" si="161"/>
+        <v>1206.3999999999999</v>
+      </c>
+      <c r="C498">
+        <f t="shared" si="162"/>
+        <v>1290.4000000000001</v>
+      </c>
+      <c r="D498">
+        <f t="shared" si="163"/>
+        <v>1464.4000000000003</v>
+      </c>
+      <c r="E498">
+        <f t="shared" si="164"/>
+        <v>1809.3999999999985</v>
+      </c>
+      <c r="F498">
+        <f t="shared" si="165"/>
+        <v>2500.8999999999987</v>
+      </c>
+      <c r="G498">
+        <f t="shared" si="166"/>
+        <v>3883.150000000006</v>
+      </c>
+      <c r="H498">
+        <f t="shared" si="167"/>
+        <v>-497.974999999994</v>
+      </c>
+      <c r="I498">
+        <f t="shared" si="168"/>
+        <v>1061.587499999976</v>
+      </c>
+      <c r="J498">
+        <f t="shared" si="169"/>
+        <v>14105.806249999976</v>
+      </c>
+      <c r="K498">
+        <f t="shared" si="170"/>
+        <v>34239.196875000096</v>
+      </c>
+    </row>
+    <row r="499" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A499">
+        <v>7</v>
+      </c>
+      <c r="B499">
+        <f t="shared" si="161"/>
+        <v>1209.3999999999999</v>
+      </c>
+      <c r="C499">
+        <f t="shared" si="162"/>
+        <v>1293.4000000000001</v>
+      </c>
+      <c r="D499">
+        <f t="shared" si="163"/>
+        <v>1467.4000000000003</v>
+      </c>
+      <c r="E499">
+        <f t="shared" si="164"/>
+        <v>1812.3999999999985</v>
+      </c>
+      <c r="F499">
+        <f t="shared" si="165"/>
+        <v>2503.8999999999987</v>
+      </c>
+      <c r="G499">
+        <f t="shared" si="166"/>
+        <v>3886.150000000006</v>
+      </c>
+      <c r="H499">
+        <f t="shared" si="167"/>
+        <v>-512.974999999994</v>
+      </c>
+      <c r="I499" s="3">
+        <f t="shared" si="168"/>
+        <v>1036.587499999976</v>
+      </c>
+      <c r="J499">
+        <f t="shared" si="169"/>
+        <v>14085.806249999976</v>
+      </c>
+      <c r="K499">
+        <f t="shared" si="170"/>
+        <v>34214.196875000096</v>
+      </c>
+    </row>
+    <row r="500" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A500">
+        <v>7</v>
+      </c>
+      <c r="B500">
+        <f t="shared" si="161"/>
+        <v>1212.3999999999999</v>
+      </c>
+      <c r="C500">
+        <f t="shared" si="162"/>
+        <v>1296.4000000000001</v>
+      </c>
+      <c r="D500">
+        <f t="shared" si="163"/>
+        <v>1470.4000000000003</v>
+      </c>
+      <c r="E500">
+        <f t="shared" si="164"/>
+        <v>1815.3999999999985</v>
+      </c>
+      <c r="F500">
+        <f t="shared" si="165"/>
+        <v>2506.8999999999987</v>
+      </c>
+      <c r="G500">
+        <f t="shared" si="166"/>
+        <v>3889.150000000006</v>
+      </c>
+      <c r="H500">
+        <f t="shared" si="167"/>
+        <v>-527.974999999994</v>
+      </c>
+      <c r="I500">
+        <f t="shared" si="168"/>
+        <v>1011.587499999976</v>
+      </c>
+      <c r="J500">
+        <f t="shared" si="169"/>
+        <v>14065.806249999976</v>
+      </c>
+      <c r="K500">
+        <f t="shared" si="170"/>
+        <v>34189.196875000096</v>
+      </c>
+    </row>
+    <row r="501" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A501">
+        <v>7</v>
+      </c>
+      <c r="B501">
+        <f t="shared" si="161"/>
+        <v>1215.3999999999999</v>
+      </c>
+      <c r="C501">
+        <f t="shared" si="162"/>
+        <v>1299.4000000000001</v>
+      </c>
+      <c r="D501">
+        <f t="shared" si="163"/>
+        <v>1473.4000000000003</v>
+      </c>
+      <c r="E501">
+        <f t="shared" si="164"/>
+        <v>1818.3999999999985</v>
+      </c>
+      <c r="F501">
+        <f t="shared" si="165"/>
+        <v>2509.8999999999987</v>
+      </c>
+      <c r="G501">
+        <f t="shared" si="166"/>
+        <v>3892.150000000006</v>
+      </c>
+      <c r="H501">
+        <f t="shared" si="167"/>
+        <v>-542.974999999994</v>
+      </c>
+      <c r="I501">
+        <f t="shared" si="168"/>
+        <v>986.58749999997599</v>
+      </c>
+      <c r="J501">
+        <f t="shared" si="169"/>
+        <v>14045.806249999976</v>
+      </c>
+      <c r="K501">
+        <f t="shared" si="170"/>
+        <v>34164.196875000096</v>
+      </c>
+    </row>
+    <row r="502" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A502">
+        <v>7</v>
+      </c>
+      <c r="B502">
+        <f t="shared" si="161"/>
+        <v>1218.3999999999999</v>
+      </c>
+      <c r="C502">
+        <f t="shared" si="162"/>
+        <v>1302.4000000000001</v>
+      </c>
+      <c r="D502">
+        <f t="shared" si="163"/>
+        <v>1476.4000000000003</v>
+      </c>
+      <c r="E502">
+        <f t="shared" si="164"/>
+        <v>1821.3999999999985</v>
+      </c>
+      <c r="F502">
+        <f t="shared" si="165"/>
+        <v>2512.8999999999987</v>
+      </c>
+      <c r="G502">
+        <f t="shared" si="166"/>
+        <v>3895.150000000006</v>
+      </c>
+      <c r="H502">
+        <f t="shared" si="167"/>
+        <v>-557.974999999994</v>
+      </c>
+      <c r="I502">
+        <f t="shared" si="168"/>
+        <v>961.58749999997599</v>
+      </c>
+      <c r="J502">
+        <f t="shared" si="169"/>
+        <v>14025.806249999976</v>
+      </c>
+      <c r="K502">
+        <f t="shared" si="170"/>
+        <v>34139.196875000096</v>
+      </c>
+    </row>
+    <row r="503" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A503">
+        <v>7</v>
+      </c>
+      <c r="B503">
+        <f t="shared" si="161"/>
+        <v>1221.3999999999999</v>
+      </c>
+      <c r="C503">
+        <f t="shared" si="162"/>
+        <v>1305.4000000000001</v>
+      </c>
+      <c r="D503">
+        <f t="shared" si="163"/>
+        <v>1479.4000000000003</v>
+      </c>
+      <c r="E503">
+        <f t="shared" si="164"/>
+        <v>1824.3999999999985</v>
+      </c>
+      <c r="F503">
+        <f t="shared" si="165"/>
+        <v>2515.8999999999987</v>
+      </c>
+      <c r="G503">
+        <f t="shared" si="166"/>
+        <v>3898.150000000006</v>
+      </c>
+      <c r="H503">
+        <f t="shared" si="167"/>
+        <v>-572.974999999994</v>
+      </c>
+      <c r="I503">
+        <f t="shared" si="168"/>
+        <v>936.58749999997599</v>
+      </c>
+      <c r="J503">
+        <f t="shared" si="169"/>
+        <v>14005.806249999976</v>
+      </c>
+      <c r="K503">
+        <f t="shared" si="170"/>
+        <v>34114.196875000096</v>
+      </c>
+    </row>
+    <row r="504" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A504">
+        <v>7</v>
+      </c>
+      <c r="B504">
+        <f t="shared" si="161"/>
+        <v>1224.3999999999999</v>
+      </c>
+      <c r="C504">
+        <f t="shared" si="162"/>
+        <v>1308.4000000000001</v>
+      </c>
+      <c r="D504">
+        <f t="shared" si="163"/>
+        <v>1482.4000000000003</v>
+      </c>
+      <c r="E504">
+        <f t="shared" si="164"/>
+        <v>1827.3999999999985</v>
+      </c>
+      <c r="F504">
+        <f t="shared" si="165"/>
+        <v>2518.8999999999987</v>
+      </c>
+      <c r="G504">
+        <f t="shared" si="166"/>
+        <v>3901.150000000006</v>
+      </c>
+      <c r="H504">
+        <f t="shared" si="167"/>
+        <v>-587.974999999994</v>
+      </c>
+      <c r="I504">
+        <f t="shared" si="168"/>
+        <v>911.58749999997599</v>
+      </c>
+      <c r="J504">
+        <f t="shared" si="169"/>
+        <v>13985.806249999976</v>
+      </c>
+      <c r="K504">
+        <f t="shared" si="170"/>
+        <v>34089.196875000096</v>
+      </c>
+    </row>
+    <row r="505" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A505">
+        <v>7</v>
+      </c>
+      <c r="B505">
+        <f t="shared" si="161"/>
+        <v>1227.3999999999999</v>
+      </c>
+      <c r="C505">
+        <f t="shared" si="162"/>
+        <v>1311.4</v>
+      </c>
+      <c r="D505">
+        <f t="shared" si="163"/>
+        <v>1485.4000000000003</v>
+      </c>
+      <c r="E505">
+        <f t="shared" si="164"/>
+        <v>1830.3999999999985</v>
+      </c>
+      <c r="F505">
+        <f t="shared" si="165"/>
+        <v>2521.8999999999987</v>
+      </c>
+      <c r="G505">
+        <f t="shared" si="166"/>
+        <v>3904.150000000006</v>
+      </c>
+      <c r="H505">
+        <f t="shared" si="167"/>
+        <v>-602.974999999994</v>
+      </c>
+      <c r="I505">
+        <f t="shared" si="168"/>
+        <v>886.58749999997599</v>
+      </c>
+      <c r="J505">
+        <f t="shared" si="169"/>
+        <v>13965.806249999976</v>
+      </c>
+      <c r="K505">
+        <f t="shared" si="170"/>
+        <v>34064.196875000096</v>
+      </c>
+    </row>
+    <row r="506" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A506">
+        <v>7</v>
+      </c>
+      <c r="B506">
+        <f t="shared" si="161"/>
+        <v>1230.3999999999999</v>
+      </c>
+      <c r="C506">
+        <f t="shared" si="162"/>
+        <v>1314.4</v>
+      </c>
+      <c r="D506">
+        <f t="shared" si="163"/>
+        <v>1488.4000000000003</v>
+      </c>
+      <c r="E506">
+        <f t="shared" si="164"/>
+        <v>1833.3999999999985</v>
+      </c>
+      <c r="F506">
+        <f t="shared" si="165"/>
+        <v>2524.8999999999987</v>
+      </c>
+      <c r="G506">
+        <f t="shared" si="166"/>
+        <v>3907.150000000006</v>
+      </c>
+      <c r="H506">
+        <f t="shared" si="167"/>
+        <v>-617.974999999994</v>
+      </c>
+      <c r="I506">
+        <f t="shared" si="168"/>
+        <v>861.58749999997599</v>
+      </c>
+      <c r="J506">
+        <f t="shared" si="169"/>
+        <v>13945.806249999976</v>
+      </c>
+      <c r="K506">
+        <f t="shared" si="170"/>
+        <v>34039.196875000096</v>
+      </c>
+    </row>
+    <row r="507" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A507">
+        <v>7</v>
+      </c>
+      <c r="B507">
+        <f t="shared" si="161"/>
+        <v>1233.3999999999999</v>
+      </c>
+      <c r="C507">
+        <f t="shared" si="162"/>
+        <v>1317.4</v>
+      </c>
+      <c r="D507">
+        <f t="shared" si="163"/>
+        <v>1491.4000000000003</v>
+      </c>
+      <c r="E507">
+        <f t="shared" si="164"/>
+        <v>1836.3999999999985</v>
+      </c>
+      <c r="F507">
+        <f t="shared" si="165"/>
+        <v>2527.8999999999987</v>
+      </c>
+      <c r="G507">
+        <f t="shared" si="166"/>
+        <v>3910.150000000006</v>
+      </c>
+      <c r="H507">
+        <f t="shared" si="167"/>
+        <v>-632.974999999994</v>
+      </c>
+      <c r="I507">
+        <f t="shared" si="168"/>
+        <v>836.58749999997599</v>
+      </c>
+      <c r="J507">
+        <f t="shared" si="169"/>
+        <v>13925.806249999976</v>
+      </c>
+      <c r="K507">
+        <f t="shared" si="170"/>
+        <v>34014.196875000096</v>
+      </c>
+    </row>
+    <row r="508" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A508">
+        <v>7</v>
+      </c>
+      <c r="B508">
+        <f t="shared" si="161"/>
+        <v>1236.3999999999999</v>
+      </c>
+      <c r="C508">
+        <f t="shared" si="162"/>
+        <v>1320.4</v>
+      </c>
+      <c r="D508">
+        <f t="shared" si="163"/>
+        <v>1494.4000000000003</v>
+      </c>
+      <c r="E508">
+        <f t="shared" si="164"/>
+        <v>1839.3999999999985</v>
+      </c>
+      <c r="F508">
+        <f t="shared" si="165"/>
+        <v>2530.8999999999987</v>
+      </c>
+      <c r="G508">
+        <f t="shared" si="166"/>
+        <v>3913.150000000006</v>
+      </c>
+      <c r="H508">
+        <f t="shared" si="167"/>
+        <v>-647.974999999994</v>
+      </c>
+      <c r="I508">
+        <f t="shared" si="168"/>
+        <v>811.58749999997599</v>
+      </c>
+      <c r="J508">
+        <f t="shared" si="169"/>
+        <v>13905.806249999976</v>
+      </c>
+      <c r="K508">
+        <f t="shared" si="170"/>
+        <v>33989.196875000096</v>
+      </c>
+    </row>
+    <row r="509" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A509">
+        <v>13</v>
+      </c>
+      <c r="B509">
+        <f t="shared" si="161"/>
+        <v>1239.3999999999999</v>
+      </c>
+      <c r="C509">
+        <f t="shared" si="162"/>
+        <v>1323.4</v>
+      </c>
+      <c r="D509">
+        <f t="shared" si="163"/>
+        <v>1497.4000000000003</v>
+      </c>
+      <c r="E509">
+        <f t="shared" si="164"/>
+        <v>1842.3999999999985</v>
+      </c>
+      <c r="F509">
+        <f t="shared" si="165"/>
+        <v>2533.8999999999987</v>
+      </c>
+      <c r="G509">
+        <f t="shared" si="166"/>
+        <v>3916.150000000006</v>
+      </c>
+      <c r="H509">
+        <f t="shared" si="167"/>
+        <v>-662.974999999994</v>
+      </c>
+      <c r="I509">
+        <f t="shared" si="168"/>
+        <v>786.58749999997599</v>
+      </c>
+      <c r="J509">
+        <f t="shared" si="169"/>
+        <v>13885.806249999976</v>
+      </c>
+      <c r="K509">
+        <f t="shared" si="170"/>
+        <v>33964.196875000096</v>
+      </c>
+    </row>
+    <row r="510" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A510">
+        <f t="shared" ref="A510" si="171">A509+3</f>
+        <v>16</v>
+      </c>
+      <c r="B510">
+        <f t="shared" si="161"/>
+        <v>1242.3999999999999</v>
+      </c>
+      <c r="C510">
+        <f t="shared" si="162"/>
+        <v>1326.4</v>
+      </c>
+      <c r="D510">
+        <f t="shared" si="163"/>
+        <v>1500.4000000000003</v>
+      </c>
+      <c r="E510">
+        <f t="shared" si="164"/>
+        <v>1845.3999999999985</v>
+      </c>
+      <c r="F510">
+        <f t="shared" si="165"/>
+        <v>2536.8999999999987</v>
+      </c>
+      <c r="G510">
+        <f t="shared" si="166"/>
+        <v>3919.150000000006</v>
+      </c>
+      <c r="H510">
+        <f t="shared" si="167"/>
+        <v>-677.974999999994</v>
+      </c>
+      <c r="I510">
+        <f t="shared" si="168"/>
+        <v>761.58749999997599</v>
+      </c>
+      <c r="J510">
+        <f t="shared" si="169"/>
+        <v>13865.806249999976</v>
+      </c>
+      <c r="K510">
+        <f t="shared" si="170"/>
+        <v>33939.196875000096</v>
+      </c>
+    </row>
+    <row r="511" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A511" s="2">
+        <v>13</v>
+      </c>
+      <c r="B511">
+        <f t="shared" si="161"/>
+        <v>1245.3999999999999</v>
+      </c>
+      <c r="C511">
+        <f t="shared" si="162"/>
+        <v>1329.4</v>
+      </c>
+      <c r="D511">
+        <f t="shared" si="163"/>
+        <v>1503.4000000000003</v>
+      </c>
+      <c r="E511">
+        <f t="shared" si="164"/>
+        <v>1848.3999999999985</v>
+      </c>
+      <c r="F511">
+        <f t="shared" si="165"/>
+        <v>2539.8999999999987</v>
+      </c>
+      <c r="G511">
+        <f t="shared" si="166"/>
+        <v>3922.150000000006</v>
+      </c>
+      <c r="H511">
+        <f t="shared" si="167"/>
+        <v>-692.974999999994</v>
+      </c>
+      <c r="I511">
+        <f t="shared" si="168"/>
+        <v>736.58749999997599</v>
+      </c>
+      <c r="J511">
+        <f t="shared" si="169"/>
+        <v>13845.806249999976</v>
+      </c>
+      <c r="K511">
+        <f t="shared" si="170"/>
+        <v>33914.196875000096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>